<commit_message>
feat(classes): implement update and deactivate class functionality with logging
</commit_message>
<xml_diff>
--- a/student-bulk-template.xlsx
+++ b/student-bulk-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29321"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Web Apps\Javascript\schomas\schomas-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B67F33-2C53-40C3-994D-A6C202F38FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F6B251-DA67-42DE-ABC2-47748A71CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>